<commit_message>
Changes in some files
</commit_message>
<xml_diff>
--- a/documentExtractionResults.xlsx
+++ b/documentExtractionResults.xlsx
@@ -533,9 +533,9 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId12"/>
-    <x:hyperlink ref="B3" r:id="rId13"/>
-    <x:hyperlink ref="B4" r:id="rId14"/>
+    <x:hyperlink ref="B2" r:id="rId9"/>
+    <x:hyperlink ref="B3" r:id="rId10"/>
+    <x:hyperlink ref="B4" r:id="rId11"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes made to the Project - changed gmail connection - Changed product updates template
</commit_message>
<xml_diff>
--- a/documentExtractionResults.xlsx
+++ b/documentExtractionResults.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A70D8-C79C-43AC-A331-70E2E4BD2FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="0" activeTab="1"/>
+    <x:workbookView xWindow="380" yWindow="980" windowWidth="14400" windowHeight="7360" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,36 +22,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <x:si>
-    <x:t>Attendees</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Agenda</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Notes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Action Items</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Next Meeting Agenda</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product, Business Development, Classroom, Execo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Last Meeting Follow-up 1. Lorem ipsum dolor sit amet, consectetuer adipiscing elit. New Business 2. Lorem ipsum dolor sit amet, consectetuer adipiscing elit. 3. Suspendisse scelerisque mi a mi.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>● Lorem ipsum dolor sit amet consectetuer adipiscing elit. ● Suspendisse scelerisque mi a mi. ● Vestibulum ante ipsum primis elementum, libero interdum auctor cursus, sapien enim dictum quam. ○ Phasellus vehicula nonummy nunc.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Lorem ipsum dolor sit amet consectetuer adipiscing elit. 2. Suspendisse scelerisque mi a mi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit.</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+  <x:si>
+    <x:t>Cybersecurity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mini-Apps</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Soft-Skills</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q1_2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Soft_skills_Strategy-linkendIn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Strategy_pilot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Strategy_1-roadmap</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Strategy_2-grade_weighting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Skills_&amp;_employability</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Learnings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mobile Development Pilot: Nucamp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Launch of the SD Mobile Course</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mpesa_Africa_Mini_Apps_Delivery</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Product_planning</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data_analytics</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Digital_marketing </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Product_Management</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Analyst</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The cybersecurity training kicked off in October 2023 as a partnership between Moringa School and ICT Authority with the goal of equipping all public servants with knowledge and fundamentals of cybersecurity. We have so far trained two cohorts from various government ministries and parastatals including the Ministry of Lands, Agricultural Finance Corporation, NCPB among others. The training consists of 7 key topics for 3 days, each 4 hours per day. The training showcased the need for cybersecurity training in government and we are looking forward to training more civil servants this year. The next cohort will commence on February 5th 2024.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Introducing our Mini Applications Development Program, a groundbreaking initiative designed for aspiring developers. This unique course, developed in collaboration with Mpesa Africa, pioneers the introduction of mini-apps on the continent, uncovering the world of cross-platform super applications. The 22-week full-time program covers front-end concepts and reactive/state programming (React) requisite to rendering multiple mobile services on a native mobile application referred to as a super-application.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Soft Skills Programme continues to be our unique selling point and as such we are constantly innovating to improve the product offering to our customers.&lt;br&gt; As of the last half of 2023 we embarked on the RFP process to get a soft skills curriculum partner who was aligned to our learning goals which is to provide an experiential learning platform. Out of the service providers who were involved in the process we settled on Turnleft Media which is a subsidiary of LinkedIn Learning in Africa. The decision was informed by the subsidized cost and the robust library of courses.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>In Q1 of 2024 and as part of the new soft skills strategy we are looking to:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Onboard students to LinkedIn Learning, a tool meant to enrich learning for our students.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>We will pilot with SDFFT 9 the 2024 soft strategy which includes:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A soft skills roadmap that will see us pace and chunk soft skills until the phase 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Implementing grade weighting of the soft skills assessments across the different phases</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Differentiating content for the skills and employability pathways</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Draw learnings from the pilot cohort and implement at scale to the rest of the 2024 cohorts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fullstack Mobile Pilot: The current React Native mobile bootcamp is designed to equip learners with the requisite skills to design cross-platform (Web &amp; Mobile) applications that can be hosted on both iOS and android app stores. The pilot entails key milestones:&lt;br&gt; Content review and Scoping: Analysis of students' journey documenting tools, services and activities required from onboarding to successful course completion.&lt;br&gt; Status: 90% : Pending Fulltime and Part-time pacing ETA 10th Feb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>In this course, you'll learn to build a mobile app using JavaScript's React Native framework. Javascript enables cross-platform software development where learners develop solutions that can be run on (compatibility with) both Android and iOS app stores.&lt;br&gt; Task: Scoping and pacing fulltime x part time schedules</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bronze module train the trainer and onboarding.&lt;br&gt; Task: Align on classroom expectations and roles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Design sprints prioritization. &lt;br&gt; Some of the courses in discussion include:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AI and Machine Learning (8-12 weeks)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Analytics (8-12 weeks)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Digital Marketing (6 weeks)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Product Management (8-12 weeks)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cybersecurity Analyst+ (22-33 weeks)</x:t>
   </x:si>
   <x:si>
     <x:t>Name</x:t>
@@ -80,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
@@ -417,14 +502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:S2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
+    <x:sheetView topLeftCell="L1" workbookViewId="0">
+      <x:selection activeCell="N1" sqref="N1"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,12 +518,17 @@
     <x:col min="2" max="2" width="35.363281" style="1" customWidth="1"/>
     <x:col min="3" max="3" width="34" style="1" customWidth="1"/>
     <x:col min="4" max="4" width="53.363281" style="1" customWidth="1"/>
-    <x:col min="5" max="5" width="18.816406" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="43.089844" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="7" max="16384" width="8.726562" style="1" customWidth="1"/>
+    <x:col min="5" max="5" width="27.542969" style="1" customWidth="1"/>
+    <x:col min="6" max="6" width="28.089844" style="1" customWidth="1"/>
+    <x:col min="7" max="7" width="8.542969" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="8" max="11" width="8.726562" style="1" customWidth="1"/>
+    <x:col min="12" max="12" width="8.726562" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="8.726562" style="1" customWidth="1"/>
+    <x:col min="14" max="14" width="8.726562" style="0" customWidth="1"/>
+    <x:col min="15" max="16384" width="8.726562" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:6" s="0" customFormat="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:19" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -454,40 +544,123 @@
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s"/>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L1" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="M1" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="N1" s="1" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O1" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P1" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Q1" s="1" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="R1" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="S1" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:6" customFormat="1" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="2" spans="1:19" customFormat="1" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C2" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E2" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G2" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="H2" s="1" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I2" s="1" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J2" s="1" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="K2" s="1" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="M2" s="1" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="O2" s="1" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="P2" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="Q2" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R2" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="S2" s="1" t="s">
+        <x:v>37</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B4"/>
+  <x:dimension ref="A1:B6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="A5" sqref="A5 5:5"/>
@@ -501,41 +674,44 @@
   <x:sheetData>
     <x:row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A1" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>13</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <x:c r="A3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>15</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <x:row r="4" spans="1:2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
-        <x:v>17</x:v>
-      </x:c>
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <x:c r="B6" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId9"/>
-    <x:hyperlink ref="B3" r:id="rId10"/>
-    <x:hyperlink ref="B4" r:id="rId11"/>
+    <x:hyperlink ref="B2" r:id="rId12"/>
+    <x:hyperlink ref="B3" r:id="rId13"/>
+    <x:hyperlink ref="B4" r:id="rId14"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>